<commit_message>
Resubo graficas e imagenes actualizadads
</commit_message>
<xml_diff>
--- a/tablas/medidas_bank.xlsx
+++ b/tablas/medidas_bank.xlsx
@@ -260,40 +260,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2475.0</v>
+        <v>2511.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3238.0</v>
+        <v>3594.0</v>
       </c>
       <c r="D5" t="n">
-        <v>33310.0</v>
+        <v>32954.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2165.0</v>
+        <v>2129.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4332224750568878</v>
+        <v>0.4113022113022113</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5334051724137931</v>
+        <v>0.5411637931034483</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9114041808033271</v>
+        <v>0.9016635657217905</v>
       </c>
       <c r="I5" t="n">
-        <v>0.4781222833961171</v>
+        <v>0.46738017682643085</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8688210158298534</v>
+        <v>0.8610517626493154</v>
       </c>
       <c r="K5" t="n">
-        <v>0.40402479763377414</v>
+        <v>0.3891878394859579</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6972429305486364</v>
+        <v>0.6985325155847683</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8373800467405629</v>
+        <v>0.8335700182187566</v>
       </c>
     </row>
     <row r="6">

</xml_diff>